<commit_message>
Se eliminan productos mansfield the Edgesupply.xlsx y Plumbingandelectric.xlsx
Estos 2 market places dejaron de vender productos de Mansfield, por lo cual se retiran dichas URL
</commit_message>
<xml_diff>
--- a/XX_Url/Edgesupply.xlsx
+++ b/XX_Url/Edgesupply.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://orgcorona-my.sharepoint.com/personal/jmonsalvo_corona_com_co/Documents/03_Proy_ID/03_MACHINE_LEARNING/01_Projects/11_Web_Scrapping/Pricing/Scrapping_git/XX_Url/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://orgcorona-my.sharepoint.com/personal/jmonsalvo_corona_com_co/Documents/03_Proy_ID/03_MACHINE_LEARNING/01_Projects/11_Web_Scrapping/00_Scrapping_git/XX_Url/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{070B33F2-2C87-45ED-92A4-C15EFB7D10ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72AFA1BC-5701-44B0-B8F3-C1ED1209B6B4}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{070B33F2-2C87-45ED-92A4-C15EFB7D10ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{492770F3-15FF-40E7-938F-BF800B982E09}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="URL" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Linea</t>
   </si>
@@ -63,18 +63,6 @@
     <t>Fabricante</t>
   </si>
   <si>
-    <t>Mansfield</t>
-  </si>
-  <si>
-    <t>103580000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BOWL 1035 EL WHT                                                                                    </t>
-  </si>
-  <si>
-    <t>https://www.edgesupply.com/Mansfield-Plumbing-103580000-White-Floor-Mount-Toilet-Bowl.HTM</t>
-  </si>
-  <si>
     <t>Gerber</t>
   </si>
   <si>
@@ -96,16 +84,7 @@
     <t>Bowl</t>
   </si>
   <si>
-    <t>VX1</t>
-  </si>
-  <si>
     <t>12</t>
-  </si>
-  <si>
-    <t>Standard</t>
-  </si>
-  <si>
-    <t>Mansfield VX1 Std EL Bowl</t>
   </si>
   <si>
     <t>Viper</t>
@@ -1031,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1058,13 +1037,13 @@
         <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -1085,7 +1064,7 @@
         <v>3</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>5</v>
@@ -1099,19 +1078,19 @@
         <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>4</v>
@@ -1120,57 +1099,16 @@
         <v>1.28</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="3">
-        <v>1.28</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{C45BCFD8-E58F-4055-BCD4-1783445531D5}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>